<commit_message>
added a script to compare IDPT SPCT and GDPT
</commit_message>
<xml_diff>
--- a/publication/analyses/outputs/supfigs/gdpt_rmse-z_by_c-min.xlsx
+++ b/publication/analyses/outputs/supfigs/gdpt_rmse-z_by_c-min.xlsx
@@ -485,7 +485,7 @@
         <v>0.4518398268398268</v>
       </c>
       <c r="G2" t="n">
-        <v>0.007172060743489314</v>
+        <v>39.76190476190476</v>
       </c>
     </row>
     <row r="3">
@@ -508,7 +508,7 @@
         <v>0.4518398268398268</v>
       </c>
       <c r="G3" t="n">
-        <v>0.007172060743489314</v>
+        <v>39.76190476190476</v>
       </c>
     </row>
     <row r="4">
@@ -531,7 +531,7 @@
         <v>0.4518398268398268</v>
       </c>
       <c r="G4" t="n">
-        <v>0.007172060743489314</v>
+        <v>39.76190476190476</v>
       </c>
     </row>
     <row r="5">
@@ -554,7 +554,7 @@
         <v>0.4518398268398268</v>
       </c>
       <c r="G5" t="n">
-        <v>0.007172060743489314</v>
+        <v>39.76190476190476</v>
       </c>
     </row>
     <row r="6">
@@ -577,7 +577,7 @@
         <v>0.4518398268398268</v>
       </c>
       <c r="G6" t="n">
-        <v>0.007172060743489314</v>
+        <v>39.76190476190476</v>
       </c>
     </row>
     <row r="7">
@@ -600,7 +600,7 @@
         <v>0.4518398268398268</v>
       </c>
       <c r="G7" t="n">
-        <v>0.007172060743489314</v>
+        <v>39.76190476190476</v>
       </c>
     </row>
     <row r="8">
@@ -623,7 +623,7 @@
         <v>0.4518398268398268</v>
       </c>
       <c r="G8" t="n">
-        <v>0.007172060743489314</v>
+        <v>39.76190476190476</v>
       </c>
     </row>
     <row r="9">
@@ -646,7 +646,7 @@
         <v>0.4518398268398268</v>
       </c>
       <c r="G9" t="n">
-        <v>0.007172060743489314</v>
+        <v>39.76190476190476</v>
       </c>
     </row>
     <row r="10">
@@ -669,7 +669,7 @@
         <v>0.4518398268398268</v>
       </c>
       <c r="G10" t="n">
-        <v>0.007172060743489314</v>
+        <v>39.76190476190476</v>
       </c>
     </row>
     <row r="11">
@@ -692,7 +692,7 @@
         <v>0.4518398268398268</v>
       </c>
       <c r="G11" t="n">
-        <v>0.007172060743489314</v>
+        <v>39.76190476190476</v>
       </c>
     </row>
     <row r="12">
@@ -715,7 +715,7 @@
         <v>0.4518398268398268</v>
       </c>
       <c r="G12" t="n">
-        <v>0.007172060743489314</v>
+        <v>39.76190476190476</v>
       </c>
     </row>
     <row r="13">
@@ -738,7 +738,7 @@
         <v>0.4518398268398268</v>
       </c>
       <c r="G13" t="n">
-        <v>0.007172060743489314</v>
+        <v>39.76190476190476</v>
       </c>
     </row>
     <row r="14">
@@ -761,7 +761,7 @@
         <v>0.4518398268398268</v>
       </c>
       <c r="G14" t="n">
-        <v>0.007172060743489314</v>
+        <v>39.76190476190476</v>
       </c>
     </row>
     <row r="15">
@@ -784,7 +784,7 @@
         <v>0.4518398268398268</v>
       </c>
       <c r="G15" t="n">
-        <v>0.007172060743489314</v>
+        <v>39.76190476190476</v>
       </c>
     </row>
     <row r="16">
@@ -807,7 +807,7 @@
         <v>0.4518398268398268</v>
       </c>
       <c r="G16" t="n">
-        <v>0.007172060743489314</v>
+        <v>39.76190476190476</v>
       </c>
     </row>
     <row r="17">
@@ -830,7 +830,7 @@
         <v>0.4518398268398268</v>
       </c>
       <c r="G17" t="n">
-        <v>0.007172060743489314</v>
+        <v>39.76190476190476</v>
       </c>
     </row>
     <row r="18">
@@ -853,7 +853,7 @@
         <v>0.4518398268398268</v>
       </c>
       <c r="G18" t="n">
-        <v>0.007172060743489314</v>
+        <v>39.76190476190476</v>
       </c>
     </row>
     <row r="19">
@@ -876,7 +876,7 @@
         <v>0.4518398268398268</v>
       </c>
       <c r="G19" t="n">
-        <v>0.007172060743489314</v>
+        <v>39.76190476190476</v>
       </c>
     </row>
     <row r="20">
@@ -899,7 +899,7 @@
         <v>0.4518398268398268</v>
       </c>
       <c r="G20" t="n">
-        <v>0.007172060743489314</v>
+        <v>39.76190476190476</v>
       </c>
     </row>
     <row r="21">
@@ -922,7 +922,7 @@
         <v>0.4518398268398268</v>
       </c>
       <c r="G21" t="n">
-        <v>0.007172060743489314</v>
+        <v>39.76190476190476</v>
       </c>
     </row>
     <row r="22">
@@ -936,7 +936,7 @@
         <v>2.079473727118974</v>
       </c>
       <c r="D22" t="n">
-        <v>2.139337574243696</v>
+        <v>2.136793603657316</v>
       </c>
       <c r="E22" t="n">
         <v>2500</v>
@@ -945,7 +945,7 @@
         <v>0.4509379509379509</v>
       </c>
       <c r="G22" t="n">
-        <v>0.007157745252983348</v>
+        <v>39.68253968253968</v>
       </c>
     </row>
     <row r="23">
@@ -959,7 +959,7 @@
         <v>2.080684736272763</v>
       </c>
       <c r="D23" t="n">
-        <v>2.139337574243696</v>
+        <v>2.136280133796781</v>
       </c>
       <c r="E23" t="n">
         <v>2494</v>
@@ -968,7 +968,7 @@
         <v>0.4498556998556998</v>
       </c>
       <c r="G23" t="n">
-        <v>0.007140566664376188</v>
+        <v>39.58730158730159</v>
       </c>
     </row>
     <row r="24">
@@ -982,7 +982,7 @@
         <v>2.082167649868273</v>
       </c>
       <c r="D24" t="n">
-        <v>2.139337574243696</v>
+        <v>2.13555450967014</v>
       </c>
       <c r="E24" t="n">
         <v>2481</v>
@@ -991,7 +991,7 @@
         <v>0.4475108225108225</v>
       </c>
       <c r="G24" t="n">
-        <v>0.007103346389060675</v>
+        <v>39.38095238095238</v>
       </c>
     </row>
     <row r="25">
@@ -1005,7 +1005,7 @@
         <v>2.082445171479229</v>
       </c>
       <c r="D25" t="n">
-        <v>2.139337574243696</v>
+        <v>2.127589679888585</v>
       </c>
       <c r="E25" t="n">
         <v>2466</v>
@@ -1014,7 +1014,7 @@
         <v>0.4448051948051948</v>
       </c>
       <c r="G25" t="n">
-        <v>0.007060399917542775</v>
+        <v>39.14285714285715</v>
       </c>
     </row>
     <row r="26">
@@ -1028,7 +1028,7 @@
         <v>2.082927480339055</v>
       </c>
       <c r="D26" t="n">
-        <v>2.139337574243696</v>
+        <v>2.127329707785147</v>
       </c>
       <c r="E26" t="n">
         <v>2463</v>
@@ -1037,7 +1037,7 @@
         <v>0.4442640692640693</v>
       </c>
       <c r="G26" t="n">
-        <v>0.007051810623239194</v>
+        <v>39.09523809523809</v>
       </c>
     </row>
     <row r="27">
@@ -1051,7 +1051,7 @@
         <v>2.081801515012496</v>
       </c>
       <c r="D27" t="n">
-        <v>2.139337574243696</v>
+        <v>2.124988642338044</v>
       </c>
       <c r="E27" t="n">
         <v>2457</v>
@@ -1060,7 +1060,7 @@
         <v>0.4431818181818182</v>
       </c>
       <c r="G27" t="n">
-        <v>0.007034632034632035</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28">
@@ -1074,7 +1074,7 @@
         <v>2.082165796058722</v>
       </c>
       <c r="D28" t="n">
-        <v>2.139337574243696</v>
+        <v>2.126195651048691</v>
       </c>
       <c r="E28" t="n">
         <v>2448</v>
@@ -1083,7 +1083,7 @@
         <v>0.4415584415584415</v>
       </c>
       <c r="G28" t="n">
-        <v>0.007008864151721294</v>
+        <v>38.85714285714285</v>
       </c>
     </row>
     <row r="29">
@@ -1097,7 +1097,7 @@
         <v>2.079737925039889</v>
       </c>
       <c r="D29" t="n">
-        <v>2.139337574243696</v>
+        <v>2.124861618068633</v>
       </c>
       <c r="E29" t="n">
         <v>2441</v>
@@ -1106,7 +1106,7 @@
         <v>0.4402958152958153</v>
       </c>
       <c r="G29" t="n">
-        <v>0.006988822465012941</v>
+        <v>38.74603174603175</v>
       </c>
     </row>
     <row r="30">
@@ -1120,7 +1120,7 @@
         <v>2.079508747247184</v>
       </c>
       <c r="D30" t="n">
-        <v>2.139337574243696</v>
+        <v>2.121556542345739</v>
       </c>
       <c r="E30" t="n">
         <v>2436</v>
@@ -1129,7 +1129,7 @@
         <v>0.4393939393939394</v>
       </c>
       <c r="G30" t="n">
-        <v>0.006974506974506974</v>
+        <v>38.66666666666666</v>
       </c>
     </row>
     <row r="31">
@@ -1143,7 +1143,7 @@
         <v>2.079053480531792</v>
       </c>
       <c r="D31" t="n">
-        <v>2.139337574243696</v>
+        <v>2.119864029668172</v>
       </c>
       <c r="E31" t="n">
         <v>2431</v>
@@ -1152,7 +1152,7 @@
         <v>0.4384920634920635</v>
       </c>
       <c r="G31" t="n">
-        <v>0.006960191484001008</v>
+        <v>38.58730158730159</v>
       </c>
     </row>
     <row r="32">
@@ -1166,7 +1166,7 @@
         <v>2.079608115701401</v>
       </c>
       <c r="D32" t="n">
-        <v>2.139337574243696</v>
+        <v>2.119958663608569</v>
       </c>
       <c r="E32" t="n">
         <v>2429</v>
@@ -1175,7 +1175,7 @@
         <v>0.4381313131313131</v>
       </c>
       <c r="G32" t="n">
-        <v>0.006954465287798622</v>
+        <v>38.55555555555556</v>
       </c>
     </row>
     <row r="33">
@@ -1189,7 +1189,7 @@
         <v>2.074153305564937</v>
       </c>
       <c r="D33" t="n">
-        <v>2.139337574243696</v>
+        <v>2.113222016897527</v>
       </c>
       <c r="E33" t="n">
         <v>2417</v>
@@ -1198,7 +1198,7 @@
         <v>0.4359668109668109</v>
       </c>
       <c r="G33" t="n">
-        <v>0.006920108110584301</v>
+        <v>38.36507936507937</v>
       </c>
     </row>
     <row r="34">
@@ -1212,7 +1212,7 @@
         <v>2.073783072430346</v>
       </c>
       <c r="D34" t="n">
-        <v>2.139337574243696</v>
+        <v>2.111660257409673</v>
       </c>
       <c r="E34" t="n">
         <v>2409</v>
@@ -1221,7 +1221,7 @@
         <v>0.4345238095238095</v>
       </c>
       <c r="G34" t="n">
-        <v>0.006897203325774755</v>
+        <v>38.23809523809524</v>
       </c>
     </row>
     <row r="35">
@@ -1235,7 +1235,7 @@
         <v>2.078419779937638</v>
       </c>
       <c r="D35" t="n">
-        <v>2.139337574243696</v>
+        <v>2.112066289773897</v>
       </c>
       <c r="E35" t="n">
         <v>2393</v>
@@ -1244,7 +1244,7 @@
         <v>0.4316378066378067</v>
       </c>
       <c r="G35" t="n">
-        <v>0.006851393756155661</v>
+        <v>37.98412698412698</v>
       </c>
     </row>
     <row r="36">
@@ -1258,7 +1258,7 @@
         <v>2.070943441783759</v>
       </c>
       <c r="D36" t="n">
-        <v>2.139337574243696</v>
+        <v>2.105810207186438</v>
       </c>
       <c r="E36" t="n">
         <v>2378</v>
@@ -1267,7 +1267,7 @@
         <v>0.4289321789321789</v>
       </c>
       <c r="G36" t="n">
-        <v>0.006808447284637761</v>
+        <v>37.74603174603175</v>
       </c>
     </row>
     <row r="37">
@@ -1281,7 +1281,7 @@
         <v>2.071295602114835</v>
       </c>
       <c r="D37" t="n">
-        <v>2.139337574243696</v>
+        <v>2.102902641161698</v>
       </c>
       <c r="E37" t="n">
         <v>2366</v>
@@ -1290,7 +1290,7 @@
         <v>0.4267676767676767</v>
       </c>
       <c r="G37" t="n">
-        <v>0.00677409010742344</v>
+        <v>37.55555555555556</v>
       </c>
     </row>
     <row r="38">
@@ -1304,7 +1304,7 @@
         <v>2.078386727720778</v>
       </c>
       <c r="D38" t="n">
-        <v>2.139337574243696</v>
+        <v>2.104468209883738</v>
       </c>
       <c r="E38" t="n">
         <v>2338</v>
@@ -1313,7 +1313,7 @@
         <v>0.4217171717171717</v>
       </c>
       <c r="G38" t="n">
-        <v>0.006693923360590028</v>
+        <v>37.11111111111111</v>
       </c>
     </row>
     <row r="39">
@@ -1327,7 +1327,7 @@
         <v>2.07149151214741</v>
       </c>
       <c r="D39" t="n">
-        <v>2.139337574243696</v>
+        <v>2.099912607935125</v>
       </c>
       <c r="E39" t="n">
         <v>2307</v>
@@ -1336,7 +1336,7 @@
         <v>0.4161255411255411</v>
       </c>
       <c r="G39" t="n">
-        <v>0.006605167319453034</v>
+        <v>36.61904761904762</v>
       </c>
     </row>
     <row r="40">
@@ -1350,7 +1350,7 @@
         <v>2.066794530592043</v>
       </c>
       <c r="D40" t="n">
-        <v>2.139337574243696</v>
+        <v>2.091878885839314</v>
       </c>
       <c r="E40" t="n">
         <v>2276</v>
@@ -1359,7 +1359,7 @@
         <v>0.4105339105339105</v>
       </c>
       <c r="G40" t="n">
-        <v>0.00651641127831604</v>
+        <v>36.12698412698413</v>
       </c>
     </row>
     <row r="41">
@@ -1373,7 +1373,7 @@
         <v>2.06039354637281</v>
       </c>
       <c r="D41" t="n">
-        <v>2.139337574243696</v>
+        <v>2.079396135689238</v>
       </c>
       <c r="E41" t="n">
         <v>2239</v>
@@ -1382,7 +1382,7 @@
         <v>0.4038600288600289</v>
       </c>
       <c r="G41" t="n">
-        <v>0.006410476648571886</v>
+        <v>35.53968253968254</v>
       </c>
     </row>
     <row r="42">
@@ -1396,7 +1396,7 @@
         <v>2.049166036997616</v>
       </c>
       <c r="D42" t="n">
-        <v>2.139337574243696</v>
+        <v>2.065359644865959</v>
       </c>
       <c r="E42" t="n">
         <v>2189</v>
@@ -1405,7 +1405,7 @@
         <v>0.3948412698412698</v>
       </c>
       <c r="G42" t="n">
-        <v>0.00626732174351222</v>
+        <v>34.74603174603175</v>
       </c>
     </row>
     <row r="43">
@@ -1419,7 +1419,7 @@
         <v>2.031196125407328</v>
       </c>
       <c r="D43" t="n">
-        <v>2.139337574243696</v>
+        <v>2.042622446870265</v>
       </c>
       <c r="E43" t="n">
         <v>2137</v>
@@ -1428,7 +1428,7 @@
         <v>0.3854617604617604</v>
       </c>
       <c r="G43" t="n">
-        <v>0.006118440642250166</v>
+        <v>33.92063492063492</v>
       </c>
     </row>
     <row r="44">
@@ -1442,7 +1442,7 @@
         <v>2.028617544163716</v>
       </c>
       <c r="D44" t="n">
-        <v>2.139337574243696</v>
+        <v>2.034839747563011</v>
       </c>
       <c r="E44" t="n">
         <v>2044</v>
@@ -1451,7 +1451,7 @@
         <v>0.3686868686868687</v>
       </c>
       <c r="G44" t="n">
-        <v>0.005852172518839185</v>
+        <v>32.44444444444444</v>
       </c>
     </row>
     <row r="45">
@@ -1465,7 +1465,7 @@
         <v>2.018705074809447</v>
       </c>
       <c r="D45" t="n">
-        <v>2.139337574243696</v>
+        <v>2.021975247708756</v>
       </c>
       <c r="E45" t="n">
         <v>1938</v>
@@ -1474,7 +1474,7 @@
         <v>0.3495670995670996</v>
       </c>
       <c r="G45" t="n">
-        <v>0.005548684120112691</v>
+        <v>30.76190476190476</v>
       </c>
     </row>
     <row r="46">
@@ -1488,7 +1488,7 @@
         <v>1.990445490551076</v>
       </c>
       <c r="D46" t="n">
-        <v>2.139337574243696</v>
+        <v>1.997742026431591</v>
       </c>
       <c r="E46" t="n">
         <v>1778</v>
@@ -1497,7 +1497,7 @@
         <v>0.3207070707070707</v>
       </c>
       <c r="G46" t="n">
-        <v>0.005090588423921757</v>
+        <v>28.22222222222222</v>
       </c>
     </row>
     <row r="47">
@@ -1511,7 +1511,7 @@
         <v>1.982498943212088</v>
       </c>
       <c r="D47" t="n">
-        <v>2.139337574243696</v>
+        <v>1.95693254851187</v>
       </c>
       <c r="E47" t="n">
         <v>1569</v>
@@ -1520,7 +1520,7 @@
         <v>0.283008658008658</v>
       </c>
       <c r="G47" t="n">
-        <v>0.004492200920772349</v>
+        <v>24.90476190476191</v>
       </c>
     </row>
     <row r="48">
@@ -1534,7 +1534,7 @@
         <v>1.91103377425726</v>
       </c>
       <c r="D48" t="n">
-        <v>2.139337574243696</v>
+        <v>1.835499263639429</v>
       </c>
       <c r="E48" t="n">
         <v>1276</v>
@@ -1543,7 +1543,7 @@
         <v>0.2301587301587301</v>
       </c>
       <c r="G48" t="n">
-        <v>0.003653313177122701</v>
+        <v>20.25396825396825</v>
       </c>
     </row>
     <row r="49">
@@ -1557,7 +1557,7 @@
         <v>1.582519106542808</v>
       </c>
       <c r="D49" t="n">
-        <v>2.139337574243696</v>
+        <v>1.504352486364895</v>
       </c>
       <c r="E49" t="n">
         <v>705</v>
@@ -1566,7 +1566,7 @@
         <v>0.1271645021645022</v>
       </c>
       <c r="G49" t="n">
-        <v>0.002018484161341305</v>
+        <v>11.19047619047619</v>
       </c>
     </row>
     <row r="50">
@@ -1580,7 +1580,7 @@
         <v>1.388206997465243</v>
       </c>
       <c r="D50" t="n">
-        <v>2.139337574243696</v>
+        <v>1.270685148540861</v>
       </c>
       <c r="E50" t="n">
         <v>170</v>
@@ -1589,7 +1589,7 @@
         <v>0.03066378066378066</v>
       </c>
       <c r="G50" t="n">
-        <v>0.0004867266772028677</v>
+        <v>2.698412698412699</v>
       </c>
     </row>
     <row r="51">
@@ -1600,9 +1600,7 @@
         <v>1</v>
       </c>
       <c r="C51" t="inlineStr"/>
-      <c r="D51" t="n">
-        <v>2.139337574243696</v>
-      </c>
+      <c r="D51" t="inlineStr"/>
       <c r="E51" t="n">
         <v>0</v>
       </c>

</xml_diff>